<commit_message>
Search by name and ID feature added
</commit_message>
<xml_diff>
--- a/server/data/employeeDetails.xlsx
+++ b/server/data/employeeDetails.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -25,15 +25,9 @@
     <t>Naga Durga Prasad</t>
   </si>
   <si>
-    <t>enagadurga.prasad@cognizant.com</t>
-  </si>
-  <si>
     <t>Eyunni Sreelatha</t>
   </si>
   <si>
-    <t>206754416@nbcu.com</t>
-  </si>
-  <si>
     <t>Thirumoorthi Sabarinathan</t>
   </si>
   <si>
@@ -43,12 +37,6 @@
     <t>Durga Vara Prasad Vadigina</t>
   </si>
   <si>
-    <t>vadiginadurga.prasad@cognizant.com</t>
-  </si>
-  <si>
-    <t>Venkata Reddy</t>
-  </si>
-  <si>
     <t>reddy.venkat@cognizant.com</t>
   </si>
   <si>
@@ -70,16 +58,40 @@
     <t>NBCU_mail</t>
   </si>
   <si>
-    <t>Sarath</t>
-  </si>
-  <si>
     <t>Sarath@cognizant.com</t>
   </si>
   <si>
-    <t>Dipansu</t>
-  </si>
-  <si>
-    <t>Theja</t>
+    <t>dipansu@cognizant.com</t>
+  </si>
+  <si>
+    <t>theja@cognizant.com</t>
+  </si>
+  <si>
+    <t>123456@nbcu.com</t>
+  </si>
+  <si>
+    <t>123455@nbcu.com</t>
+  </si>
+  <si>
+    <t>123457@nbcu.com</t>
+  </si>
+  <si>
+    <t>Dipansu Ruwatia</t>
+  </si>
+  <si>
+    <t>Theja Vadla</t>
+  </si>
+  <si>
+    <t>Sarath Kumar</t>
+  </si>
+  <si>
+    <t>Venkata Reddy Vuyyuru</t>
+  </si>
+  <si>
+    <t>ndp@cognizant.com</t>
+  </si>
+  <si>
+    <t>v.prasad@cognizant.com</t>
   </si>
 </sst>
 </file>
@@ -449,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,204 +479,200 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>2249636</v>
+        <v>12345</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>206754416</v>
+        <v>54321</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>2249637</v>
+        <v>12346</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>206754417</v>
+        <v>54322</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>2249638</v>
+        <v>12347</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>206754418</v>
+        <v>54323</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>2249639</v>
+        <v>12348</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>206754419</v>
+        <v>54324</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>2249640</v>
+        <v>12349</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>206754420</v>
+        <v>54325</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>2249641</v>
+        <v>12350</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>54326</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
-      </c>
-      <c r="D7">
-        <v>206754421</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>2249642</v>
+        <v>12351</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>206754422</v>
+        <v>54327</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>2249643</v>
+        <v>12352</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>206754423</v>
+        <v>54328</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C4" r:id="rId4"/>
-    <hyperlink ref="C5" r:id="rId5"/>
-    <hyperlink ref="C6" r:id="rId6"/>
-    <hyperlink ref="F3" r:id="rId7"/>
-    <hyperlink ref="F4" r:id="rId8"/>
-    <hyperlink ref="F5" r:id="rId9"/>
-    <hyperlink ref="F6" r:id="rId10"/>
-    <hyperlink ref="C7" r:id="rId11"/>
-    <hyperlink ref="C8" r:id="rId12"/>
-    <hyperlink ref="F7" r:id="rId13"/>
-    <hyperlink ref="F8" r:id="rId14"/>
-    <hyperlink ref="C9" r:id="rId15"/>
-    <hyperlink ref="F9" r:id="rId16"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>